<commit_message>
fixed error in signs
</commit_message>
<xml_diff>
--- a/support/2024.xlsx
+++ b/support/2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rcoc-my.sharepoint.com/personal/abates_rcoc_org/Documents/Desktop/Bids/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rcoc-my.sharepoint.com/personal/abates_rcoc_org/Documents/Documents/GitHub/bidAnalysis/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{DFD50A24-B97B-44C6-AEB4-97FC5F00CCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88247D0C-883F-4853-8E41-00067F086753}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{DFD50A24-B97B-44C6-AEB4-97FC5F00CCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54FD3460-BC35-4F33-A1F7-8327060F4937}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -321,7 +321,7 @@
     </r>
   </si>
   <si>
-    <t>Item</t>
+    <t>Item Number</t>
   </si>
 </sst>
 </file>
@@ -590,6 +590,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -597,6 +606,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -608,25 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1000,180 +1000,180 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="30" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="20" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="20" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="22"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="22"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="20" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="20" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="20" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="20" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="22"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="29" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="20" t="s">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="22"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="20">
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="23">
         <v>50</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="20" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="22"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="20" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="20" t="s">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="22"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1316,201 +1316,201 @@
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:13" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="28">
+      <c r="F18" s="20">
         <v>30620</v>
       </c>
-      <c r="G18" s="28"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="12"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="28">
+      <c r="K18" s="20">
         <v>34855.5</v>
       </c>
-      <c r="L18" s="28"/>
+      <c r="L18" s="20"/>
       <c r="M18" s="14"/>
     </row>
     <row r="20" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="30" t="s">
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="20" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="20" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="22"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="20" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="20" t="s">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="22"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="32">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26">
         <v>1000</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="22"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="20" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="22"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="20" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="20">
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="23">
         <v>25</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="22"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="20" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="20" t="s">
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="22"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="22"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -1665,43 +1665,54 @@
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:13" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="28">
+      <c r="F33" s="20">
         <v>46943.6</v>
       </c>
-      <c r="G33" s="28"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="14"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
-      <c r="K33" s="28">
+      <c r="K33" s="20">
         <v>58394.75</v>
       </c>
-      <c r="L33" s="28"/>
+      <c r="L33" s="20"/>
       <c r="M33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="I21:M21"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="I24:M24"/>
-    <mergeCell ref="I25:M25"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="I23:M23"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="I11:M11"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="I6:M6"/>
     <mergeCell ref="A18:C18"/>
@@ -1718,33 +1729,22 @@
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="I22:M22"/>
-    <mergeCell ref="I23:M23"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="I25:M25"/>
     <mergeCell ref="I26:M26"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="F33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
@@ -1760,7 +1760,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,6 +2765,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="668c7407-b5b1-42b7-9c16-29d46fcfc2cb" xsi:nil="true"/>
@@ -2773,15 +2782,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2986,20 +2986,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3FFF2E-744B-40D2-B9A5-C744F2979CD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4AE3917-73D0-418E-A4DF-B12993C79B58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="668c7407-b5b1-42b7-9c16-29d46fcfc2cb"/>
     <ds:schemaRef ds:uri="396adcb7-f279-4b24-a21a-a75d7dd8678e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3FFF2E-744B-40D2-B9A5-C744F2979CD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>